<commit_message>
updated till 40 + fixed some issues-
</commit_message>
<xml_diff>
--- a/test/Finished/地点.xlsx
+++ b/test/Finished/地点.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\线上校庆\All\RICOH THETA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\My Drive\线上校庆\All\RICOH THETA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A38D01BE-3E3B-4B2A-8FA4-DC0F85BEADB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A831427-1BBF-4938-BA6D-EDA9AB4AE4AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3040659-2446-41D9-B5E2-0089247F2668}"/>
+    <workbookView xWindow="10035" yWindow="0" windowWidth="9000" windowHeight="6600" xr2:uid="{B3040659-2446-41D9-B5E2-0089247F2668}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="157">
   <si>
     <t>门口1</t>
   </si>
@@ -97,6 +98,411 @@
   </si>
   <si>
     <t>JK楼走道4</t>
+  </si>
+  <si>
+    <t>JK楼走道5</t>
+  </si>
+  <si>
+    <t>K楼左侧楼梯</t>
+  </si>
+  <si>
+    <t>K101前门</t>
+  </si>
+  <si>
+    <t>K102后面K103前门</t>
+  </si>
+  <si>
+    <t>K103中间</t>
+  </si>
+  <si>
+    <t>K103后门K104前门</t>
+  </si>
+  <si>
+    <t>K104中间</t>
+  </si>
+  <si>
+    <t>K104后门K105前门</t>
+  </si>
+  <si>
+    <t>K101中间</t>
+  </si>
+  <si>
+    <t>K101后门K102前门</t>
+  </si>
+  <si>
+    <t>K102中间</t>
+  </si>
+  <si>
+    <t>K105中间</t>
+  </si>
+  <si>
+    <t>K105后门K106前门</t>
+  </si>
+  <si>
+    <t>K106后门</t>
+  </si>
+  <si>
+    <t>K楼右侧楼梯</t>
+  </si>
+  <si>
+    <t>K楼到体育馆走道</t>
+  </si>
+  <si>
+    <t>Container办公室</t>
+  </si>
+  <si>
+    <t>进入体育馆楼梯</t>
+  </si>
+  <si>
+    <t>体育馆入口1</t>
+  </si>
+  <si>
+    <t>体育馆入口2</t>
+  </si>
+  <si>
+    <t>体育馆中央</t>
+  </si>
+  <si>
+    <t>测量体温点</t>
+  </si>
+  <si>
+    <t>体育馆出口1</t>
+  </si>
+  <si>
+    <t>体育馆出口2</t>
+  </si>
+  <si>
+    <t>体育馆通往体育处楼梯</t>
+  </si>
+  <si>
+    <t>楼梯口</t>
+  </si>
+  <si>
+    <t>通往体育处</t>
+  </si>
+  <si>
+    <t>侧楼讲堂通道</t>
+  </si>
+  <si>
+    <t>体育处储藏室</t>
+  </si>
+  <si>
+    <t>镜鸿楼走道</t>
+  </si>
+  <si>
+    <t>镜鸿楼1楼楼梯</t>
+  </si>
+  <si>
+    <t>镜鸿楼2楼楼梯</t>
+  </si>
+  <si>
+    <t>镜鸿楼3楼楼梯</t>
+  </si>
+  <si>
+    <t>镜鸿楼4楼楼梯</t>
+  </si>
+  <si>
+    <t>C410前面</t>
+  </si>
+  <si>
+    <t>C410后面C411后面</t>
+  </si>
+  <si>
+    <t>C411中间</t>
+  </si>
+  <si>
+    <t>C411前面C412前面C413前面</t>
+  </si>
+  <si>
+    <t>C412后面C413中间</t>
+  </si>
+  <si>
+    <t>C415前面C413后面</t>
+  </si>
+  <si>
+    <t>C415后面</t>
+  </si>
+  <si>
+    <t>侧楼4楼通往食堂3楼</t>
+  </si>
+  <si>
+    <t>通往侧楼4楼和上食堂4楼下食堂2楼</t>
+  </si>
+  <si>
+    <t>通往侧楼3楼和上食堂3楼下食堂</t>
+  </si>
+  <si>
+    <t>C313&amp;C314后面</t>
+  </si>
+  <si>
+    <t>C313&amp;C314中间</t>
+  </si>
+  <si>
+    <t>C311&amp;C312后面</t>
+  </si>
+  <si>
+    <t>C311&amp;C312前面</t>
+  </si>
+  <si>
+    <t>C309后面</t>
+  </si>
+  <si>
+    <t>C308中间</t>
+  </si>
+  <si>
+    <t>C308前面</t>
+  </si>
+  <si>
+    <t>物理室后面，分子生物室</t>
+  </si>
+  <si>
+    <t>物理室中间</t>
+  </si>
+  <si>
+    <t>物理室前面</t>
+  </si>
+  <si>
+    <t>生物室，化学室前面</t>
+  </si>
+  <si>
+    <t>生物室，化学室后面</t>
+  </si>
+  <si>
+    <t>通往食堂2楼和侧楼1楼</t>
+  </si>
+  <si>
+    <t>食堂1</t>
+  </si>
+  <si>
+    <t>食堂2</t>
+  </si>
+  <si>
+    <t>食堂3</t>
+  </si>
+  <si>
+    <t>食堂4</t>
+  </si>
+  <si>
+    <t>食堂5</t>
+  </si>
+  <si>
+    <t>食堂6</t>
+  </si>
+  <si>
+    <t>食堂7</t>
+  </si>
+  <si>
+    <t>食堂8</t>
+  </si>
+  <si>
+    <t>食堂9</t>
+  </si>
+  <si>
+    <t>食堂10</t>
+  </si>
+  <si>
+    <t>食堂11</t>
+  </si>
+  <si>
+    <t>食堂12</t>
+  </si>
+  <si>
+    <t>通往宽友楼</t>
+  </si>
+  <si>
+    <t>食堂右侧底楼楼梯</t>
+  </si>
+  <si>
+    <t>食堂左侧底楼楼梯</t>
+  </si>
+  <si>
+    <t>通往食堂2楼和敬业楼</t>
+  </si>
+  <si>
+    <t>食堂右侧2楼楼梯楼</t>
+  </si>
+  <si>
+    <t>食堂右侧3楼楼梯楼</t>
+  </si>
+  <si>
+    <t>食堂左侧2楼楼梯</t>
+  </si>
+  <si>
+    <t>B201后面</t>
+  </si>
+  <si>
+    <t>B201中间</t>
+  </si>
+  <si>
+    <t>B201前面B202后面</t>
+  </si>
+  <si>
+    <t>B202中间</t>
+  </si>
+  <si>
+    <t>B202前面</t>
+  </si>
+  <si>
+    <t>B203后面</t>
+  </si>
+  <si>
+    <t>B203中间</t>
+  </si>
+  <si>
+    <t>B204前面</t>
+  </si>
+  <si>
+    <t>B204中间</t>
+  </si>
+  <si>
+    <t>B204后面</t>
+  </si>
+  <si>
+    <t>B205中间</t>
+  </si>
+  <si>
+    <t>B205后面</t>
+  </si>
+  <si>
+    <t>B206前面</t>
+  </si>
+  <si>
+    <t>B206后面</t>
+  </si>
+  <si>
+    <t>B307前面</t>
+  </si>
+  <si>
+    <t>B307中间</t>
+  </si>
+  <si>
+    <t>B307后面B306后面</t>
+  </si>
+  <si>
+    <t>B306前面</t>
+  </si>
+  <si>
+    <t>B305前面</t>
+  </si>
+  <si>
+    <t>B304前面</t>
+  </si>
+  <si>
+    <t>B303前面</t>
+  </si>
+  <si>
+    <t>B302前面</t>
+  </si>
+  <si>
+    <t>B302中间</t>
+  </si>
+  <si>
+    <t>B302后面B301前面</t>
+  </si>
+  <si>
+    <t>B301中间</t>
+  </si>
+  <si>
+    <t>B301后面 食堂左侧3楼梯口</t>
+  </si>
+  <si>
+    <t>食堂3楼和4楼之间的楼梯</t>
+  </si>
+  <si>
+    <t>食堂左侧4楼梯 音乐室后面</t>
+  </si>
+  <si>
+    <t>音乐室中间1</t>
+  </si>
+  <si>
+    <t>音乐室中间2</t>
+  </si>
+  <si>
+    <t>音乐室前面</t>
+  </si>
+  <si>
+    <t>B402前面</t>
+  </si>
+  <si>
+    <t>B402中间</t>
+  </si>
+  <si>
+    <t>B403前面B404后面</t>
+  </si>
+  <si>
+    <t>B404中间</t>
+  </si>
+  <si>
+    <t>B404前面</t>
+  </si>
+  <si>
+    <t>食堂右侧4楼梯</t>
+  </si>
+  <si>
+    <t>通往食堂3楼</t>
+  </si>
+  <si>
+    <t>食堂通往宽友楼1</t>
+  </si>
+  <si>
+    <t>食堂通往宽友楼2</t>
+  </si>
+  <si>
+    <t>食堂通往宽友楼3</t>
+  </si>
+  <si>
+    <t>烹饪室前面</t>
+  </si>
+  <si>
+    <t>敬业右侧中间1</t>
+  </si>
+  <si>
+    <t>敬业右侧中间2</t>
+  </si>
+  <si>
+    <t>敬业右侧中间3</t>
+  </si>
+  <si>
+    <t>敬业右侧中间4</t>
+  </si>
+  <si>
+    <t>敬业楼底楼楼梯</t>
+  </si>
+  <si>
+    <t>接着6从门口上来</t>
+  </si>
+  <si>
+    <t>通往141</t>
+  </si>
+  <si>
+    <t>通往草场</t>
+  </si>
+  <si>
+    <t>草场左侧</t>
+  </si>
+  <si>
+    <t>草场中间</t>
+  </si>
+  <si>
+    <t>草场右侧</t>
+  </si>
+  <si>
+    <t>通往146上去畹香楼</t>
+  </si>
+  <si>
+    <t>从141接着上来</t>
+  </si>
+  <si>
+    <t>通往畹香楼走道1</t>
+  </si>
+  <si>
+    <t>通往畹香楼走道2</t>
+  </si>
+  <si>
+    <t>通往畹香楼走道3</t>
+  </si>
+  <si>
+    <t>通往畹香楼走道4</t>
   </si>
 </sst>
 </file>
@@ -454,18 +860,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE54A172-E3A6-4686-BE6B-060E4499832E}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -473,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -481,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -489,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -497,7 +904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -505,15 +912,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -521,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -529,7 +939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -537,7 +947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -545,7 +955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -553,7 +963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -561,7 +971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -569,7 +979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -577,7 +987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -585,7 +995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -593,7 +1003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -601,7 +1011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -609,7 +1019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -617,7 +1027,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -625,7 +1035,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -633,7 +1043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -641,28 +1051,1537 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>129</v>
+      </c>
+      <c r="B129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>131</v>
+      </c>
+      <c r="B131" t="s">
+        <v>134</v>
+      </c>
+      <c r="C131" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>132</v>
+      </c>
+      <c r="B132" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>135</v>
+      </c>
+      <c r="B135" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>137</v>
+      </c>
+      <c r="B137" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>145</v>
+      </c>
+      <c r="C141" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>150</v>
+      </c>
+      <c r="B150" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44E67EC-B985-4F1A-89FC-6F9D2511AC4B}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="B1:C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="C38">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="C39">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="C41">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="C42">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="C43">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="C44">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C45">
+    <sortCondition ref="C1:C45"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>